<commit_message>
feat: finish some steps
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,10 +458,15 @@
           <t>work_hours</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>week</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45000</v>
+        <v>45012</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -477,11 +482,14 @@
         <is>
           <t>00:00:09</t>
         </is>
+      </c>
+      <c r="E2" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45000</v>
+        <v>45012</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -497,11 +505,14 @@
         <is>
           <t>00:00:02</t>
         </is>
+      </c>
+      <c r="E3" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45000</v>
+        <v>45012</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -510,18 +521,21 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>11:16:51</t>
+          <t>22:40:55</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>00:01:13</t>
-        </is>
+          <t>11:25:17</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45000</v>
+        <v>45012</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -537,11 +551,14 @@
         <is>
           <t>00:02:17</t>
         </is>
+      </c>
+      <c r="E5" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45000</v>
+        <v>45012</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -557,11 +574,14 @@
         <is>
           <t>00:00:08</t>
         </is>
+      </c>
+      <c r="E6" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45000</v>
+        <v>45012</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -570,18 +590,21 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>11:22:42</t>
+          <t>22:40:55</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>00:00:16</t>
-        </is>
+          <t>11:18:29</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45000</v>
+        <v>45012</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -597,11 +620,14 @@
         <is>
           <t>00:00:02</t>
         </is>
+      </c>
+      <c r="E8" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45000</v>
+        <v>45012</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -617,11 +643,14 @@
         <is>
           <t>00:01:08</t>
         </is>
+      </c>
+      <c r="E9" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45000</v>
+        <v>45012</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -630,18 +659,21 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>11:31:39</t>
+          <t>22:40:55</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>00:03:11</t>
-        </is>
+          <t>11:12:27</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45000</v>
+        <v>45012</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -657,11 +689,14 @@
         <is>
           <t>00:00:09</t>
         </is>
+      </c>
+      <c r="E11" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45000</v>
+        <v>45012</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -677,11 +712,14 @@
         <is>
           <t>00:00:59</t>
         </is>
+      </c>
+      <c r="E12" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45000</v>
+        <v>45012</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -697,11 +735,14 @@
         <is>
           <t>00:00:29</t>
         </is>
+      </c>
+      <c r="E13" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45000</v>
+        <v>45012</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -717,11 +758,14 @@
         <is>
           <t>00:00:17</t>
         </is>
+      </c>
+      <c r="E14" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45000</v>
+        <v>45012</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -730,18 +774,21 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>11:40:55</t>
+          <t>22:40:55</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>00:01:29</t>
-        </is>
+          <t>11:01:29</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45000</v>
+        <v>45012</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -757,11 +804,14 @@
         <is>
           <t>00:00:47</t>
         </is>
+      </c>
+      <c r="E16" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45000</v>
+        <v>45012</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -777,11 +827,14 @@
         <is>
           <t>00:03:20</t>
         </is>
+      </c>
+      <c r="E17" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45000</v>
+        <v>45012</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -797,11 +850,14 @@
         <is>
           <t>00:00:02</t>
         </is>
+      </c>
+      <c r="E18" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45000</v>
+        <v>45012</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -810,18 +866,21 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>11:50:05</t>
+          <t>22:40:55</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>00:00:01</t>
-        </is>
+          <t>10:50:51</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45000</v>
+        <v>45011</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -837,11 +896,14 @@
         <is>
           <t>00:03:26</t>
         </is>
+      </c>
+      <c r="E20" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45000</v>
+        <v>45012</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -857,11 +919,14 @@
         <is>
           <t>00:00:32</t>
         </is>
+      </c>
+      <c r="E21" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45000</v>
+        <v>45013</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -870,13 +935,16 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>12:13:35</t>
+          <t>17:40:35</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>00:00:06</t>
-        </is>
+          <t>05:27:06</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>